<commit_message>
version 1.1, adding make mail for request, russian name in files
</commit_message>
<xml_diff>
--- a/data/Реестр выполненных работ (Перерегистрация ККТ с заменой  ФН).xlsx
+++ b/data/Реестр выполненных работ (Перерегистрация ККТ с заменой  ФН).xlsx
@@ -5,23 +5,26 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shilke\PycharmProjects\skill_set\programming\python\report_util\gr\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shilke\Desktop\Новая папка - улула\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="perereg_on_fn" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Дата</t>
+  </si>
+  <si>
+    <t>09.03.2021</t>
   </si>
   <si>
     <t>Наименование</t>
@@ -287,32 +290,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -384,6 +388,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,359 +674,361 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I4"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23:I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="5" max="6" width="9.109375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="10" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="32" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="32" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="18"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="29"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-    </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="29"/>
+    </row>
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="29"/>
+    </row>
+    <row r="12" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>1</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="12" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>1</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="B13" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
         <v>2</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="B14" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
         <v>3</v>
       </c>
-      <c r="B15" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="B15" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
         <v>4</v>
       </c>
-      <c r="B16" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+      <c r="B16" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
         <v>5</v>
       </c>
-      <c r="B17" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="B17" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="12"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="12"/>
+    <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="12"/>
+    <row r="20" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="12"/>
+    <row r="21" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="20" t="s">
+    <row r="22" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>

</xml_diff>